<commit_message>
Fix visualization scripts to work with updated master df.
</commit_message>
<xml_diff>
--- a/_reference_data/nps_park_sites_api.xlsx
+++ b/_reference_data/nps_park_sites_api.xlsx
@@ -666,12 +666,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Aleutian Islands World War II National Monument</t>
+          <t>Aleutian Islands World War II National Historic Area</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>National Monument</t>
+          <t>National Historic Area</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -8108,7 +8108,7 @@
       </c>
       <c r="D281" t="inlineStr">
         <is>
-          <t>ID,IL,IA,KS,MO,MT,NE,ND,OR,SD,WA</t>
+          <t>IA,ID,IL,IN,KS,KY,MO,MT,NE,ND,OH,OR,PA,SD,WA,WV</t>
         </is>
       </c>
       <c r="E281" t="n">

</xml_diff>